<commit_message>
added new features and improved prompts
</commit_message>
<xml_diff>
--- a/src/assets/Diccionario_datos.xlsx
+++ b/src/assets/Diccionario_datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauth\OneDrive\Desktop\open_ai_assistant_v2\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626047D6-0893-4BB3-8B73-2457CEB604F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73160FB-C83F-47DB-A749-877295ECF15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="7992" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EC975475-3123-4B78-8A3F-346E00D8290E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC975475-3123-4B78-8A3F-346E00D8290E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="216">
   <si>
     <t>Tabla</t>
   </si>
@@ -246,60 +246,12 @@
 	[Estado] [VARCHAR](10) NOT NULL)</t>
   </si>
   <si>
-    <t>CREATE TABLE IF NOT EXISTS dbo_v2.flu_tipo_fluido (
-    Id INT PRIMARY KEY,
-    Nombre VARCHAR(100),
-    Abreviatura VARCHAR(100),
-    Estado VARCHAR(100)
-)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 CREATE TABLE IF NOT EXISTS  [dbo_v2].[med_tipo_medicion](
 	[Id] [INT] IDENTITY(8,1) NOT NULL,
 	[Nombre] [VARCHAR](150) NOT NULL,
 	[NombreArbol] [VARCHAR](150) NULL,
 	[Estado] [VARCHAR](10) NOT NULL)</t>
-  </si>
-  <si>
-    <t>CREATE TABLE  IF NOT EXISTS [dbo_v2].[med_sistema_medicion](
-	[Id] [INT] IDENTITY(1,1) NOT NULL,
-	[IdPlataforma_fk] [INT] NOT NULL,
-	[Nombre] [VARCHAR](150) NOT NULL,
-	[Tag] [VARCHAR](50) NOT NULL,
-	[Estado] [VARCHAR](10) NOT NULL,
-	[FechaInicialMuestreo] [DATE] NULL,
-	[IdCliente] [INT] NOT NULL,
-	[IdTipoFluido_fk] [INT] NOT NULL,
-	[SubTipoFluido] [VARCHAR](10) NULL,
-	[IdAplicabilidad_fk] [INT] NOT NULL,
-	[SHOW_AUTOMATIC] [BIT] NULL,
-	[VarCromatografia] [INT] NULL,
-	[Prover] [BIT] NULL,
-	[IsDisponible] [BIT] NULL,
-	[IdMeteringStation_fk] [INT] NULL,
-	[IdClase_fk] [INT] NULL,
-	[SamplingPointTag] [VARCHAR](15) NULL,
-	[LimiteEstadisticoInicial] [DECIMAL](10, 5) NULL,	
-	[RefPid] [VARCHAR](200) NULL,
-	[NumeroLineaProceso] [VARCHAR](200) NULL,
-	[Localizacion] [VARCHAR](200) NULL,
-	[NominalLineSize] [VARCHAR](200) NULL,
-	[IdSchedule_fk] [INT] NULL,
-	[IdRating_fk] [INT] NULL,
-	[ClasificacionArea] [VARCHAR](200) NULL,
-	[Servicio] [VARCHAR](200) NULL,
-	[LimiteEstadistico_Default] [BIT] NULL,
-	[LimiteEstadistico_Manual] [DECIMAL](18, 2) NULL,
-	[IdSamplingPoint_fk] [INT] NULL,
-	[IsVisible] [BIT] NOT NULL
-	[Uso] [VARCHAR](50) NULL,
-	[IdArea_fk] [INT] NULL,
-	[NombreSanqGas] [VARCHAR](50) NULL,
-	[IdDeBaseOperacional_fk] [INT] NULL,
-	[EsProvador] [BIT] NULL,
-	[Tramo] [VARCHAR](50) NULL,
-	[IdDelSistemaAsociado_fk] [INT] NULL)</t>
   </si>
   <si>
     <t>CREATE TABLE  IF NOT EXISTS [dbo_v2].[fcs_tipo_dato](
@@ -346,70 +298,6 @@
 	[IdFirmware_fk] [INT] NULL)</t>
   </si>
   <si>
-    <t>CREATE TABLE IF NOT EXISTS [dbo_v2].[fcs_computadores](
-	[Id] [INT] IDENTITY(1,1) NOT NULL,
-	[IP] [VARCHAR](30) NULL,
-	[Puerto] [INT] NULL,
-	[Puerto_Secundario] [INT] NULL,
-	[Id_Modbus] [INT] NULL,
-	[Id_Modbus_Secundario] [INT] NULL,
-	[Tag] [VARCHAR](50) NULL,
-	[Compatibilidad_Modicon] [BIT] NULL,
-	[Id_Computador_Redundante] [INT] NULL,
-	[Estado] [INT] NULL,
-	[Master] [BIT] NULL,
-	[Usuario] [VARCHAR](50) NULL,
-	[Contraseña] [VARCHAR](50) NULL,
-	[Leer_Tiempo_Real] [BIT] NULL,
-	[Leer_Configuracion] [BIT] NULL,
-	[Leer_Alarmas] [BIT] NULL,
-	[Leer_Eventos] [BIT] NULL,
-	[Leer_Historicos] [BIT] NULL,
-	[Grupo_Destino] [INT] NULL,
-	[Unidad_Destino] [INT] NULL,
-	[Grupo_Fuente] [INT] NULL,
-	[Unidad_Fuente] [INT] NULL,
-	[Orden_Archivos] [INT] NULL,
-	[Numero_Maximo_Horarios] [INT] NULL,
-	[Numero_Maximo_Diarios] [INT] NULL,
-	[Numero_Maximo_Proves] [INT] NULL,
-	[Numero_Maximo_Batch] [INT] NULL,
-	[Tipo_Protocolo] [INT] NULL,
-	[Tiempo_Proceso_Historico] [INT] NULL,
-	[Tiempo_Proceso_TiempoReal] [INT] NULL,
-	[IdFirmware_fk] [INT] NULL,
-	[IdEquipo_fk] [INT] NULL,
-	[Servidor_OPC] [VARCHAR](50) NULL)</t>
-  </si>
-  <si>
-    <t>CREATE TABLE IF NOT EXISTS  [dbo_v2].[fcs_computador_medidor](
-	[Id] [INT] IDENTITY(1,1) NOT NULL,
-	[Codigo_Medidor] [INT] NULL,
-	[Estado] [VARCHAR](10) NULL,
-	[Id_Sisema_Medicion] [INT] NULL,
-	[Id_Sistema_Medicion_Redundante] [INT] NULL,	
-	[IdComputador_fk] [INT] NULL)</t>
-  </si>
-  <si>
-    <t>CREATE TABLE IF NOT EXISTS [dbo_v2].[var_tipo_variable](
-	[Id] [INT] IDENTITY(91,1) NOT NULL,
-	[Nombre] [VARCHAR](150) NOT NULL,
-	[Reporte_Manual] [BIT] NULL,
-	[IdRepManual] [INT] NULL,
-	[Id_Field] [VARCHAR](3) NULL,
-	[Cromatografia] [BIT] NULL,
-	[Estado] [VARCHAR](10) NOT NULL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-CREATE TABLE IF NOT EXISTS [dbo_v2].[var_variable_datos](
-	[Fecha] [DATE] NOT NULL,
-	[idVariable_fk] [INT] NOT NULL,
-	[idSistemaMedicion_fk] [INT] NOT NULL,
-	[Valor] [DECIMAL](18, 6) NULL,
-	[Valor_String] [VARCHAR](100) NULL)</t>
-  </si>
-  <si>
     <t>platform,instalation,station</t>
   </si>
   <si>
@@ -420,12 +308,6 @@
   </si>
   <si>
     <t>variable types,process variables</t>
-  </si>
-  <si>
-    <t>measurement system,fluid,fluid type,fluids,gas,oleo,water,liquid,measurement types,platform,instalation,station,receptionpoint,delivery point,measurement point,metering system</t>
-  </si>
-  <si>
-    <t>firmware,computer types,flow computer brand,brand,manufacturer,revision</t>
   </si>
   <si>
     <t>modbus map,firmware,computer types,flow computer brand,brand,manufacturer,revision,data types,point types</t>
@@ -554,9 +436,6 @@
 )</t>
   </si>
   <si>
-    <t>Codigo_2</t>
-  </si>
-  <si>
     <t>When user asks about 'Gross flow' use 'Vazão Bruta' in the WHERE statement instead</t>
   </si>
   <si>
@@ -925,9 +804,6 @@
     <t>The table flu_tipo_fluido contains the types of fluids used in the application. For example: Gás Natural, Óleo Cru y Água</t>
   </si>
   <si>
-    <t>The table med_sistema_medicion It contains the measurement systems, they can be identified by the Name or Tag. Additionally, there is the type of fluid, the type of measurement of the measurement system and the installation to which it belongs. With the SubTypeFluid column you can obtain if the measurement system is Differential Gas = DIF or linear gas = LIN</t>
-  </si>
-  <si>
     <t>The table fcs_computadores They contain the equipment that can be read. The name is found in the Tag column. Each device has a relationship with the firmware.</t>
   </si>
   <si>
@@ -938,6 +814,61 @@
   </si>
   <si>
     <t>The table var_variable_datos contains the results of the execution of the variables for each measurement system. They are classified by the measurement system through the idSistemaMedicion_fk column and the variable through the idVariable_fk column.'</t>
+  </si>
+  <si>
+    <t>List of versions</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT f.firmware
+FROM dbo_v2.fcs_firmware f;</t>
+  </si>
+  <si>
+    <t>When user asks about computer types,flow computer brand,brand,manufacturer,revision he refers to firmware</t>
+  </si>
+  <si>
+    <t>The table med_sistema_medicion It contains the measurement systems, they can be identified by the Name or Tag. Additionally, there is the type of fluid, the type of measurement of the measurement system and the installation to which it belongs. With the SubTypeFluid column you can obtain if the measurement system is Differential Gas = DIF or linear gas = LIN. The status of a measurement system is INA or ACT</t>
+  </si>
+  <si>
+    <t>measurement system,fluid,fluid type,fluids,gas,oleo,water,liquid,measurement types,platform,instalation,station,reception point,delivery point,measurement point,metering system</t>
+  </si>
+  <si>
+    <t>Palabras clave_2</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>fluid</t>
+  </si>
+  <si>
+    <t>measurement system</t>
+  </si>
+  <si>
+    <t>measurement types,fiscal, apropriação,operacional,custódia y poços de produção</t>
+  </si>
+  <si>
+    <t>firmware,equipment configuration,revision</t>
+  </si>
+  <si>
+    <t>computer type</t>
+  </si>
+  <si>
+    <t>modus map</t>
+  </si>
+  <si>
+    <t>firmware</t>
+  </si>
+  <si>
+    <t>flow computer</t>
+  </si>
+  <si>
+    <t>flow computer,measurement system</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
+    <t>variables type</t>
   </si>
 </sst>
 </file>
@@ -953,12 +884,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -1105,7 +1042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1131,59 +1068,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1519,105 +1462,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4F017C-7EC3-4C56-B817-0674D91135B0}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="36" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="54.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="83.44140625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="32.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="36" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="4.21875" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="21.21875" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="54.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="152.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>75</v>
+      <c r="B2" s="7" t="s">
+        <v>204</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>76</v>
+      <c r="B3" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1625,420 +1570,446 @@
         <v>56</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="1" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+    <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="14">
+        <v>7</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="10">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="H12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="12">
-        <v>2</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="3">
-        <v>3</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="17" t="s">
+      <c r="H13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="13">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21">
-        <v>1</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="H14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="22">
-        <v>7</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="12">
-        <v>8</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="3">
-        <v>5</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21">
-        <v>6</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>82</v>
+      <c r="B15" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="7">
         <v>8</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="I15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="J15" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="12">
+      <c r="G16" s="10">
         <v>10</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="H16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="I16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21">
+      <c r="J16" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="13">
         <v>4</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="H17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="I17" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="10">
+        <v>4</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="141" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="12">
-        <v>4</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21">
+    </row>
+    <row r="20" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="13">
         <v>12</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="H20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="I20" s="15" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="21" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F12:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2048,592 +2019,603 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4553A9B0-BF4C-4B26-9913-BBE85F52A98A}">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="76.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="58" style="26" customWidth="1"/>
-    <col min="4" max="4" width="118" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="26" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B92" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B99" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B100" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="104" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="25"/>
+      <c r="A104" s="16"/>
     </row>
     <row r="105" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: added new features
</commit_message>
<xml_diff>
--- a/src/assets/Diccionario_datos.xlsx
+++ b/src/assets/Diccionario_datos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauth\OneDrive\Desktop\open_ai_assistant_v2\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73160FB-C83F-47DB-A749-877295ECF15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDB8424-C7F5-468A-99B5-29D464DAFED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC975475-3123-4B78-8A3F-346E00D8290E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{EC975475-3123-4B78-8A3F-346E00D8290E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Vanna_info" sheetId="2" r:id="rId2"/>
+    <sheet name="Context" sheetId="3" r:id="rId2"/>
+    <sheet name="Vanna" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
   <si>
     <t>Tabla</t>
   </si>
@@ -243,14 +244,6 @@
 	[CNPJ] [VARCHAR](MAX) NULL,
 	[Abreviatura] [VARCHAR](50) NULL,
 	[EsVisible] [BIT] NOT NULL,
-	[Estado] [VARCHAR](10) NOT NULL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-CREATE TABLE IF NOT EXISTS  [dbo_v2].[med_tipo_medicion](
-	[Id] [INT] IDENTITY(8,1) NOT NULL,
-	[Nombre] [VARCHAR](150) NOT NULL,
-	[NombreArbol] [VARCHAR](150) NULL,
 	[Estado] [VARCHAR](10) NOT NULL)</t>
   </si>
   <si>
@@ -869,6 +862,145 @@
   </si>
   <si>
     <t>variables type</t>
+  </si>
+  <si>
+    <t>Descriptions</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS  [dbo_v2].[med_tipo_medicion](
+	[Id] [INT] IDENTITY(8,1) NOT NULL,
+	[Nombre] [VARCHAR](150) NOT NULL,
+	[NombreArbol] [VARCHAR](150) NULL,
+	[Estado] [VARCHAR](10) NOT NULL)</t>
+  </si>
+  <si>
+    <t>tables</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>ddls</t>
+  </si>
+  <si>
+    <t>descriptions</t>
+  </si>
+  <si>
+    <t>The table fcs_computadores contain the equipment/flow computers that can be read. The name is found in the Tag column. Each device has a relationship with the firmware.</t>
+  </si>
+  <si>
+    <t>The table fcs_firmware contains firmware/configuration/revision types used by the devices that can be read. A device can have 1 or more types of configuration or firmware.</t>
+  </si>
+  <si>
+    <t>The table fcs_mapa_modbus contains the data structure that can be read from a computer. There are relations to other tables: fcs_tipo_dato to obtain the type of the data, fcs_firmware to obtain which firmware it belongs to.</t>
+  </si>
+  <si>
+    <t>The table fcs_tipo_computador contains the different types/models/brands of equipment that can be read. Types can be OMNI, KHRONE, ROC, FC302.</t>
+  </si>
+  <si>
+    <t>The table fcs_tipos_punto contains the structure of the data that can be read by an ROC type device.</t>
+  </si>
+  <si>
+    <t>The table fcs_tipo_dato contains the types of data used to read the devices. These can be of type FLOAT, ASCII, Double.</t>
+  </si>
+  <si>
+    <t>The table med_tipo_medicion contains the measurement types of measurement systems. For explample: Fiscal, Apropriação, Operacional, Custódia y Poços de Produção.</t>
+  </si>
+  <si>
+    <t>The table flu_tipo_fluido contains the types of fluids used in the application. For example: Gás Natural, Óleo Cru y Água.</t>
+  </si>
+  <si>
+    <t>The table pla_plataforma contains information of all installations registered in the database.</t>
+  </si>
+  <si>
+    <t>The table var_tipo_variable contains the type/name of variables. For example: diferential pressure, frequency,temperature, static pressure, flow net,flow rate per day,flow NSV,volume net,volume IV,volume NSV (m3).</t>
+  </si>
+  <si>
+    <t>The table med_sistema_medicion It contains the measurement systems, they can be identified by the Name or Tag. Here is able to ask for the type of fluid, the type of measurement of the measurement system and the installation to which it belongs.  Also is able to ask for SubTypeFluid column you can obtain if the measurement system is Differential Gas = DIF or linear gas = LIN. Also could ask the status of a measurement system is INA or ACT.</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS dbo_v2.pla_plataforma(
+	Id INT PRIMARY KEY,
+	IdTipoPlataforma_fk INT ,
+	IdCliente_fk INT ,
+	Nombre VARCHAR(MAX) ,
+	Codigo VARCHAR(10) NULL,
+	CNPJ VARCHAR(MAX) NULL,
+	Abreviatura VARCHAR(50) NULL,
+	EsVisible BIT ,
+	Estado VARCHAR(10) )</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS  dbo_v2.med_tipo_medicion(
+	Id INT PRIMARY KEY,
+	Nombre VARCHAR(150) ,
+	NombreArbol VARCHAR(150),
+	Estado VARCHAR(10) )</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS dbo_v2.fcs_tipos_punto(
+	Id INT PRIMARY KEY,
+	Tipo_Punto INT ,
+	Parametro INT ,
+	Acceso VARCHAR(50) ,
+	Descripcion VARCHAR(MAX) ,
+	Tipo_Dato VARCHAR(50) ,
+	Numero_Bytes INT )</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS dbo_v2.fcs_tipo_computador(
+	Id INT PRIMARY KEY ,
+	Nombre VARCHAR(50) ,
+	Estado VARCHAR(10) )</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS dbo_v2.fcs_firmware(
+	Id INT PRIMARY KEY ,
+	Firmware VARCHAR(100) ,
+	Estado VARCHAR(10) ,	
+	IdTipo_Computador_fk INT ,
+        FOREIGN KEY (IdTipo_Computador_fk) 
+REFERENCES dbo_v2.fcs_tipo_computador (Id))</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS dbo_v2.fcs_mapa_modbus(
+	Id INT PRIMARY KEY,
+	Tag VARCHAR(MAX) ,
+	Tag_Index INT ,
+	Tag_OPC VARCHAR(MAX) ,
+	Registro INT ,
+	Punto INT ,
+	Numero_Logico INT ,
+	Funcion_Modbus INT ,
+	IdTipoDato_fk INT ,
+	IdTipos_Punto_fk INT ,
+	IdFirmware_fk INT,
+        FOREIGN KEY (IdFirmware_fk) REFERENCES dbo_v2.fcs_firmware (Id),
+        FOREIGN KEY (IdTipoDato_fk) REFERENCES dbo_v2.fcs_tipo_dato (Id),
+        FOREIGN KEY (IdTipos_Punto_fk) REFERENCES dbo_v2.fcs_tipos_punto (Id) )</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS  dbo_v2.fcs_tipo_dato(
+	Id INT PRIMARY KEY,
+	Tipo VARCHAR(100)  ,
+	Bytes INT  ,
+	Estado VARCHAR(5) )</t>
+  </si>
+  <si>
+    <t>The fcs_computador_medidor table connect fcs_computadores table and med_sistema_medicion with IdComputador_fk that is a foreign key referencing the Id column in the fcs_computadores table and the Id_Sisema_Medicion is a foreign key referencing the Id column in the med_sistema_medicion table.
+You can find info about meters for each measurement system, the flow computer to which it is a part is found in the column idcomputer_fk.</t>
+  </si>
+  <si>
+    <t>The table var_variable_datos contains read/measured/calculated values for variables in table var_tipo_variable.</t>
+  </si>
+  <si>
+    <t>When user asks about a question and there is no table related in the database information, answer with 'No SELECT statement could be found in the SQL code'</t>
+  </si>
+  <si>
+    <t>When user asks a question and there are missing parameters in question, answer with 'No SELECT statement could be found in the SQL code'</t>
+  </si>
+  <si>
+    <t>Human is asking for a list of measurement systems</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1081,6 +1213,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1091,6 +1226,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1117,15 +1261,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1462,107 +1597,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4F017C-7EC3-4C56-B817-0674D91135B0}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F12" sqref="F12:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="32.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="36" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="4.21875" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="21.21875" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="54.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="4" width="46.6640625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="36" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="21.21875" style="3" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="54.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="19" t="s">
         <v>59</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="K1" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1570,92 +1711,94 @@
         <v>56</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="D5" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="F5" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="10">
         <v>2</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="3">
+      <c r="K5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="C6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="J6" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="13">
+    <row r="7" spans="1:11" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="14">
         <v>1</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:11" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1664,24 +1807,25 @@
       <c r="C8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="G8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1690,416 +1834,666 @@
       <c r="C9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="G9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="1" t="s">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="11" spans="1:11" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="15">
+        <v>7</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="K11" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="C12" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="H12" s="10">
+        <v>8</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="14" t="s">
+      <c r="K12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="C13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="3">
         <v>5</v>
       </c>
-      <c r="G11" s="14">
-        <v>7</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="10">
-        <v>8</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="3">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="J13" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="13">
+    <row r="14" spans="1:11" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="14">
         <v>6</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="7">
+        <v>8</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="C16" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="7">
+      <c r="H16" s="10">
+        <v>10</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="14">
+        <v>4</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="10">
-        <v>10</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="13">
-        <v>4</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="F19" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="G19" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="10">
+      <c r="H19" s="10">
         <v>4</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="I19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="J19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="13">
+      <c r="K19" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="14">
         <v>12</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="I20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="J20" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:11" ht="100.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="100.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90ACFCD-A70A-4264-AF00-4E35D476ED85}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="54.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="19"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4553A9B0-BF4C-4B26-9913-BBE85F52A98A}">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="55.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="36.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41" style="2" customWidth="1"/>
+    <col min="5" max="6" width="57" style="2" customWidth="1"/>
     <col min="7" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2107,515 +2501,527 @@
         <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B57" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B59" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B61" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="62" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B64" s="1" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B64" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B66" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B66" s="1" t="s">
+    <row r="67" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B67" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B67" s="1" t="s">
+    <row r="68" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B68" s="1" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B68" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B70" s="1" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B70" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="71" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B72" s="1" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B72" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="73" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B74" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B74" s="1" t="s">
+    <row r="75" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B75" s="1" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B75" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="76" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B77" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B77" s="1" t="s">
+    <row r="78" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B78" s="1" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B78" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="79" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B80" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B80" s="1" t="s">
+    <row r="81" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B81" s="1" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B84" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B84" s="1" t="s">
+    <row r="85" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B85" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B85" s="1" t="s">
+    <row r="86" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B86" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B86" s="1" t="s">
+    <row r="87" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B87" s="1" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B87" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="88" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B89" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B89" s="1" t="s">
+    <row r="90" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B90" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B90" s="1" t="s">
+    <row r="91" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B91" s="1" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B91" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B92" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B93" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B93" s="1" t="s">
+    <row r="94" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B94" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B94" s="1" t="s">
+    <row r="95" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B95" s="1" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B95" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="96" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B97" s="1" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B97" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B99" s="1" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B99" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="104" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="16"/>
+      <c r="A104" s="17"/>
     </row>
     <row r="105" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>